<commit_message>
Inserido Fluxos de Eventos que faltavam, corrigido atores do UCP e criado o template do Sistema Web
</commit_message>
<xml_diff>
--- a/Modela/User Case Points - UCP.xlsx
+++ b/Modela/User Case Points - UCP.xlsx
@@ -663,7 +663,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -674,7 +674,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +789,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,7 +810,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="6">
         <f>B12*C12+B13*C13+B14*C14</f>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
       </c>
       <c r="B18" s="3">
         <f>C8+C15</f>
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B54" s="3">
         <f>B18*D37*D51</f>
-        <v>37.555199999999999</v>
+        <v>41.467199999999991</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B56" s="3">
         <f>B54*B55</f>
-        <v>751.10400000000004</v>
+        <v>829.34399999999982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>